<commit_message>
Add capitolo 2 - clearer CLV example
</commit_message>
<xml_diff>
--- a/16_Basic_Customer_Lifetime_value.xlsx
+++ b/16_Basic_Customer_Lifetime_value.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/Code/IULM/IULM_DDM2324_Notebooks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/Code/DDM_2425/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E96C76F8-AF5D-3541-89AC-28485B5E6404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A90C05A6-05B7-314E-9A8C-A0C60F3BE1DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{1D489133-C4D1-43E9-A6C5-92547F21AB1A}"/>
+    <workbookView xWindow="940" yWindow="2020" windowWidth="33860" windowHeight="17500" xr2:uid="{1D489133-C4D1-43E9-A6C5-92547F21AB1A}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic CLV Model" sheetId="1" r:id="rId1"/>
@@ -211,7 +211,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>=(1/(1+$C$3)^(D9-1))</t>
+          <t>=(1/(1+$C$3)^D9)</t>
         </r>
       </text>
     </comment>
@@ -474,7 +474,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -514,13 +514,14 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -977,7 +978,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D2F3B1B-84CF-47B0-BADE-11BAF9835DA6}">
-  <dimension ref="B1:Q43"/>
+  <dimension ref="B1:Y43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
@@ -996,16 +997,16 @@
     <col min="12" max="12" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:25" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="9">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
@@ -1013,7 +1014,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:25" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
@@ -1021,22 +1022,22 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="6" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:25" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
-      <c r="M6" s="21" t="s">
+      <c r="M6" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="N6" s="21"/>
-      <c r="O6" s="21"/>
-      <c r="P6" s="21"/>
-      <c r="Q6" s="21"/>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="N6" s="22"/>
+      <c r="O6" s="22"/>
+      <c r="P6" s="22"/>
+      <c r="Q6" s="22"/>
+    </row>
+    <row r="7" spans="2:25" x14ac:dyDescent="0.2">
       <c r="B7" s="13" t="s">
         <v>9</v>
       </c>
@@ -1054,11 +1055,11 @@
       </c>
       <c r="I7" s="18">
         <f>SUMPRODUCT(E8:E43,F8:F43)/C2</f>
-        <v>5.8713529426394153</v>
+        <v>5.8713529426394144</v>
       </c>
       <c r="L7" s="15">
         <f>I9</f>
-        <v>293.56764713197077</v>
+        <v>293.56764713197072</v>
       </c>
       <c r="M7" s="14">
         <v>0.05</v>
@@ -1075,14 +1076,20 @@
       <c r="Q7" s="14">
         <v>0.14000000000000001</v>
       </c>
-    </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="T7" s="24"/>
+      <c r="U7" s="14"/>
+      <c r="V7" s="14"/>
+      <c r="W7" s="14"/>
+      <c r="X7" s="14"/>
+      <c r="Y7" s="14"/>
+    </row>
+    <row r="8" spans="2:25" x14ac:dyDescent="0.2">
       <c r="D8" s="1">
         <v>0</v>
       </c>
       <c r="E8" s="8">
         <f>$C$2*($C$4^D8)</f>
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="F8" s="7">
         <f>(1/(1+$C$3)^D8)</f>
@@ -1094,7 +1101,7 @@
       <c r="I8" s="19">
         <v>50</v>
       </c>
-      <c r="K8" s="22" t="s">
+      <c r="K8" s="23" t="s">
         <v>11</v>
       </c>
       <c r="L8" s="14">
@@ -1111,22 +1118,23 @@
         <v>109.86012602963442</v>
       </c>
       <c r="P8" s="16">
-        <v>107.57998947851355</v>
+        <v>107.57998947851357</v>
       </c>
       <c r="Q8" s="16">
-        <v>105.46494235188175</v>
-      </c>
-    </row>
-    <row r="9" spans="2:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+        <v>105.46494235188177</v>
+      </c>
+      <c r="T8" s="14"/>
+    </row>
+    <row r="9" spans="2:25" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D9" s="1">
         <v>1</v>
       </c>
       <c r="E9" s="8">
-        <f t="shared" ref="E9:E43" si="0">$C$2*($C$4^D9)</f>
-        <v>95</v>
+        <f t="shared" ref="E9:E18" si="0">$C$2*($C$4^D9)</f>
+        <v>0.95</v>
       </c>
       <c r="F9" s="7">
-        <f t="shared" ref="F9:F43" si="1">(1/(1+$C$3)^D9)</f>
+        <f t="shared" ref="F9:F18" si="1">(1/(1+$C$3)^D9)</f>
         <v>0.90909090909090906</v>
       </c>
       <c r="H9" s="4" t="s">
@@ -1134,73 +1142,75 @@
       </c>
       <c r="I9" s="20">
         <f>I7*I8</f>
-        <v>293.56764713197077</v>
-      </c>
-      <c r="K9" s="22"/>
+        <v>293.56764713197072</v>
+      </c>
+      <c r="K9" s="23"/>
       <c r="L9" s="14">
         <v>0.7</v>
       </c>
       <c r="M9" s="16">
-        <v>148.2658470084167</v>
+        <v>148.26584700841667</v>
       </c>
       <c r="N9" s="16">
-        <v>140.90015148529824</v>
+        <v>140.90015148529827</v>
       </c>
       <c r="O9" s="16">
-        <v>136.54706867903346</v>
+        <v>136.54706867903343</v>
       </c>
       <c r="P9" s="16">
         <v>132.57542108185589</v>
       </c>
       <c r="Q9" s="16">
-        <v>128.93935039963583</v>
-      </c>
-    </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.2">
+        <v>128.93935039963586</v>
+      </c>
+      <c r="T9" s="14"/>
+    </row>
+    <row r="10" spans="2:25" x14ac:dyDescent="0.2">
       <c r="D10" s="1">
         <v>2</v>
       </c>
       <c r="E10" s="8">
         <f t="shared" si="0"/>
-        <v>90.25</v>
+        <v>0.90249999999999997</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="1"/>
         <v>0.82644628099173545</v>
       </c>
-      <c r="K10" s="22"/>
+      <c r="K10" s="23"/>
       <c r="L10" s="14">
         <v>0.8</v>
       </c>
       <c r="M10" s="16">
-        <v>199.45305061384605</v>
+        <v>199.45305061384596</v>
       </c>
       <c r="N10" s="16">
         <v>185.75213970341471</v>
       </c>
       <c r="O10" s="16">
-        <v>177.81368060235971</v>
+        <v>177.81368060235968</v>
       </c>
       <c r="P10" s="16">
-        <v>170.67854837079904</v>
+        <v>170.67854837079901</v>
       </c>
       <c r="Q10" s="16">
-        <v>164.23958576417027</v>
-      </c>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.2">
+        <v>164.23958576417024</v>
+      </c>
+      <c r="T10" s="14"/>
+    </row>
+    <row r="11" spans="2:25" x14ac:dyDescent="0.2">
       <c r="D11" s="1">
         <v>3</v>
       </c>
       <c r="E11" s="8">
         <f t="shared" si="0"/>
-        <v>85.737499999999983</v>
+        <v>0.85737499999999989</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="1"/>
         <v>0.75131480090157754</v>
       </c>
-      <c r="K11" s="22"/>
+      <c r="K11" s="23"/>
       <c r="L11" s="14">
         <v>0.9</v>
       </c>
@@ -1211,28 +1221,29 @@
         <v>259.62360427753856</v>
       </c>
       <c r="O11" s="16">
-        <v>244.75310763140482</v>
+        <v>244.75310763140476</v>
       </c>
       <c r="P11" s="16">
-        <v>231.58213334101069</v>
+        <v>231.58213334101063</v>
       </c>
       <c r="Q11" s="16">
         <v>219.86490298818478</v>
       </c>
-    </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="T11" s="14"/>
+    </row>
+    <row r="12" spans="2:25" x14ac:dyDescent="0.2">
       <c r="D12" s="1">
         <v>4</v>
       </c>
       <c r="E12" s="8">
         <f t="shared" si="0"/>
-        <v>81.450625000000002</v>
+        <v>0.81450624999999999</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="1"/>
         <v>0.68301345536507052</v>
       </c>
-      <c r="K12" s="22"/>
+      <c r="K12" s="23"/>
       <c r="L12" s="14">
         <v>0.95</v>
       </c>
@@ -1243,67 +1254,68 @@
         <v>314.05211585983687</v>
       </c>
       <c r="O12" s="16">
-        <v>293.56764713197077</v>
+        <v>293.56764713197072</v>
       </c>
       <c r="P12" s="16">
         <v>275.54752744607686</v>
       </c>
       <c r="Q12" s="16">
-        <v>259.62360427753845</v>
-      </c>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.2">
+        <v>259.6236042775385</v>
+      </c>
+      <c r="T12" s="14"/>
+    </row>
+    <row r="13" spans="2:25" x14ac:dyDescent="0.2">
       <c r="D13" s="1">
         <v>5</v>
       </c>
       <c r="E13" s="8">
         <f t="shared" si="0"/>
-        <v>77.378093750000005</v>
+        <v>0.77378093749999999</v>
       </c>
       <c r="F13" s="7">
         <f t="shared" si="1"/>
         <v>0.62092132305915493</v>
       </c>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:25" x14ac:dyDescent="0.2">
       <c r="D14" s="1">
         <v>6</v>
       </c>
       <c r="E14" s="8">
         <f t="shared" si="0"/>
-        <v>73.509189062499985</v>
+        <v>0.73509189062499991</v>
       </c>
       <c r="F14" s="7">
         <f t="shared" si="1"/>
         <v>0.56447393005377722</v>
       </c>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:25" x14ac:dyDescent="0.2">
       <c r="D15" s="1">
         <v>7</v>
       </c>
       <c r="E15" s="8">
         <f t="shared" si="0"/>
-        <v>69.833729609374998</v>
+        <v>0.69833729609374995</v>
       </c>
       <c r="F15" s="7">
         <f t="shared" si="1"/>
         <v>0.51315811823070645</v>
       </c>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:25" x14ac:dyDescent="0.2">
       <c r="D16" s="1">
         <v>8</v>
       </c>
       <c r="E16" s="8">
         <f t="shared" si="0"/>
-        <v>66.342043128906241</v>
+        <v>0.66342043128906247</v>
       </c>
       <c r="F16" s="7">
         <f t="shared" si="1"/>
         <v>0.46650738020973315</v>
       </c>
-      <c r="K16" s="23" t="s">
+      <c r="K16" s="21" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1313,7 +1325,7 @@
       </c>
       <c r="E17" s="8">
         <f t="shared" si="0"/>
-        <v>63.024940972460932</v>
+        <v>0.6302494097246093</v>
       </c>
       <c r="F17" s="7">
         <f t="shared" si="1"/>
@@ -1329,7 +1341,7 @@
       </c>
       <c r="E18" s="8">
         <f t="shared" si="0"/>
-        <v>59.873693923837891</v>
+        <v>0.5987369392383789</v>
       </c>
       <c r="F18" s="7">
         <f t="shared" si="1"/>

</xml_diff>